<commit_message>
Update Covid Dose Ver 2
</commit_message>
<xml_diff>
--- a/Immunizations.xlsx
+++ b/Immunizations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marmarti\Documents\Github\pcc-immtrac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053D1F69-9D92-4773-A8B4-012BD5046DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9F953E-6224-4198-ADE8-EF3FE280E303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update pcc refresh page
</commit_message>
<xml_diff>
--- a/Immunizations.xlsx
+++ b/Immunizations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marmarti\Documents\Github\pcc-immtrac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981049FF-8B84-472D-ABA4-B37FE8474F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41321BEC-548F-45ED-8863-B6FF48C0369C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="169">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -509,6 +509,39 @@
   </si>
   <si>
     <t>Boostrix</t>
+  </si>
+  <si>
+    <t>azdhsId</t>
+  </si>
+  <si>
+    <t>vacc35_1</t>
+  </si>
+  <si>
+    <t>vacc34_1</t>
+  </si>
+  <si>
+    <t>vacc26_1</t>
+  </si>
+  <si>
+    <t>vacc22_1</t>
+  </si>
+  <si>
+    <t>vacc18_1</t>
+  </si>
+  <si>
+    <t>vacc15_1</t>
+  </si>
+  <si>
+    <t>vacc10_1</t>
+  </si>
+  <si>
+    <t>vacc8_1</t>
+  </si>
+  <si>
+    <t>vacc38_1</t>
+  </si>
+  <si>
+    <t>vacc39_1</t>
   </si>
 </sst>
 </file>
@@ -904,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,15 +954,15 @@
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" customWidth="1"/>
-    <col min="13" max="13" width="112.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="112.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -961,25 +994,28 @@
         <v>149</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>93</v>
       </c>
@@ -1010,24 +1046,27 @@
       <c r="J2" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="9">
+      <c r="N2" s="2"/>
+      <c r="O2" s="9">
         <v>1</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>2</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>101</v>
       </c>
@@ -1058,26 +1097,29 @@
       <c r="J3" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>1</v>
       </c>
-      <c r="O3" s="9">
+      <c r="P3" s="9">
         <v>20</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>129</v>
       </c>
@@ -1108,26 +1150,29 @@
       <c r="J4" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="N4" s="9">
+      <c r="O4" s="9">
         <v>1</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <v>160</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>107</v>
       </c>
@@ -1158,26 +1203,29 @@
       <c r="J5" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="9">
+      <c r="O5" s="9">
         <v>1</v>
       </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
         <v>60</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>109</v>
       </c>
@@ -1208,24 +1256,27 @@
       <c r="J6" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="9">
+      <c r="N6" s="2"/>
+      <c r="O6" s="9">
         <v>1</v>
       </c>
-      <c r="O6" s="10">
+      <c r="P6" s="10">
         <v>1</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -1256,26 +1307,29 @@
       <c r="J7" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N7" s="9">
+      <c r="O7" s="9">
         <v>1</v>
       </c>
-      <c r="O7" s="10">
+      <c r="P7" s="10">
         <v>51</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>115</v>
       </c>
@@ -1306,26 +1360,29 @@
       <c r="J8" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="N8" s="10">
+      <c r="O8" s="10">
         <v>3</v>
       </c>
-      <c r="O8" s="10">
+      <c r="P8" s="10">
         <v>22</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>120</v>
       </c>
@@ -1356,26 +1413,29 @@
       <c r="J9" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="N9" s="9">
+      <c r="O9" s="9">
         <v>1</v>
       </c>
-      <c r="O9" s="10">
+      <c r="P9" s="10">
         <v>40</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1406,26 +1466,29 @@
       <c r="J10" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="N10" s="10">
+      <c r="O10" s="10">
         <v>1</v>
       </c>
-      <c r="O10" s="10">
+      <c r="P10" s="10">
         <v>30</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>78</v>
       </c>
@@ -1456,24 +1519,27 @@
       <c r="J11" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="10">
+      <c r="N11" s="2"/>
+      <c r="O11" s="10">
         <v>1</v>
       </c>
-      <c r="O11" s="10">
+      <c r="P11" s="10">
         <v>8</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>126</v>
       </c>
@@ -1504,26 +1570,29 @@
       <c r="J12" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N12" s="10">
+      <c r="O12" s="10">
         <v>1</v>
       </c>
-      <c r="O12" s="10">
+      <c r="P12" s="10">
         <v>232</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>126</v>
       </c>
@@ -1554,22 +1623,25 @@
       <c r="J13" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="N13" s="10">
+      <c r="O13" s="10">
         <v>1</v>
       </c>
-      <c r="O13" s="10">
+      <c r="P13" s="10">
         <v>232</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert AZDHS to use lot number
</commit_message>
<xml_diff>
--- a/Immunizations.xlsx
+++ b/Immunizations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\pcc-immtrac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7E26F8-8666-4AFD-BE2C-23FC34D39A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F3A71-21C4-4B20-9715-020A173B7465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -986,7 +986,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>